<commit_message>
updated admin page & server
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12983386-23AE-48B6-B79D-F4752FFFF810}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC0BADF-508F-4049-AB8F-5025E72C4FF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Тестовый отдел" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -466,12 +466,12 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -509,1597 +509,1598 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(0,100000)</f>
-        <v>94072</v>
+        <v>6571</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:M2" ca="1" si="0">RANDBETWEEN(0,100000)</f>
-        <v>65152</v>
+        <v>37829</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>1373</v>
+        <v>81348</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>93507</v>
+        <v>71395</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>9057</v>
+        <v>90533</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>21061</v>
+        <v>7402</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>30040</v>
+        <v>66895</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>67970</v>
+        <v>42083</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>29632</v>
+        <v>84861</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>60582</v>
+        <v>25087</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>39723</v>
+        <v>73797</v>
       </c>
       <c r="M2">
         <f t="shared" ca="1" si="0"/>
-        <v>17902</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>52934</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:M31" ca="1" si="1">RANDBETWEEN(0,100000)</f>
-        <v>62646</v>
+        <v>95867</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>90976</v>
+        <v>6611</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>69924</v>
+        <v>45109</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>2487</v>
+        <v>80210</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>58563</v>
+        <v>40128</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>76648</v>
+        <v>96737</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>61420</v>
+        <v>40426</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="1"/>
-        <v>80245</v>
+        <v>82588</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="1"/>
-        <v>99849</v>
+        <v>55402</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="1"/>
-        <v>70492</v>
+        <v>51551</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="1"/>
-        <v>51483</v>
+        <v>28583</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="1"/>
-        <v>12054</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>88121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>91467</v>
+        <v>30919</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>62818</v>
+        <v>78329</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>56294</v>
+        <v>140</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>76408</v>
+        <v>19828</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>51261</v>
+        <v>42686</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>70780</v>
+        <v>98021</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>93865</v>
+        <v>92582</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="1"/>
-        <v>32330</v>
+        <v>16444</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="1"/>
-        <v>60197</v>
+        <v>80979</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="1"/>
-        <v>7365</v>
+        <v>11268</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="1"/>
-        <v>2422</v>
+        <v>7582</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="1"/>
-        <v>45159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>74035</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>68104</v>
+        <v>36380</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>32267</v>
+        <v>55895</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>43167</v>
+        <v>34421</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>13958</v>
+        <v>58419</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>91266</v>
+        <v>1518</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>63223</v>
+        <v>31334</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>944</v>
+        <v>70036</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="1"/>
-        <v>29121</v>
+        <v>66929</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="1"/>
-        <v>12242</v>
+        <v>6455</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="1"/>
-        <v>82599</v>
+        <v>55187</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="1"/>
-        <v>72358</v>
+        <v>565</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="1"/>
-        <v>42931</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>9832</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>78287</v>
+        <v>66703</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>91292</v>
+        <v>49131</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>12557</v>
+        <v>35620</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>1995</v>
+        <v>78681</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>99783</v>
+        <v>42473</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>71295</v>
+        <v>95219</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>25064</v>
+        <v>80083</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="1"/>
-        <v>81557</v>
+        <v>10481</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="1"/>
-        <v>22569</v>
+        <v>50044</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="1"/>
-        <v>29968</v>
+        <v>32647</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="1"/>
-        <v>94886</v>
+        <v>43196</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="1"/>
-        <v>62329</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3383</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>67479</v>
+        <v>69908</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>55295</v>
+        <v>52906</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>47791</v>
+        <v>43976</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>14956</v>
+        <v>58760</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>32475</v>
+        <v>96108</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>16891</v>
+        <v>43225</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>99683</v>
+        <v>10395</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="1"/>
-        <v>69717</v>
+        <v>22582</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>41047</v>
+        <v>77978</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="1"/>
-        <v>60909</v>
+        <v>66699</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="1"/>
-        <v>26507</v>
+        <v>89085</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="1"/>
-        <v>98178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>59836</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>73369</v>
+        <v>81465</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>18530</v>
+        <v>5495</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>49304</v>
+        <v>81244</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>83409</v>
+        <v>64285</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>9107</v>
+        <v>20734</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>23335</v>
+        <v>53085</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>27733</v>
+        <v>64279</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="1"/>
-        <v>38473</v>
+        <v>86060</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="1"/>
-        <v>57197</v>
+        <v>54952</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="1"/>
-        <v>77900</v>
+        <v>64302</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="1"/>
-        <v>53408</v>
+        <v>80672</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="1"/>
-        <v>80676</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>41337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>87651</v>
+        <v>55017</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>61074</v>
+        <v>14321</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>41217</v>
+        <v>86684</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>47426</v>
+        <v>69946</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>24523</v>
+        <v>50853</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
+        <v>81153</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="1"/>
+        <v>6693</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="1"/>
+        <v>13046</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ca="1" si="1"/>
         <v>12013</v>
       </c>
-      <c r="H9">
-        <f t="shared" ca="1" si="1"/>
-        <v>36909</v>
-      </c>
-      <c r="I9">
-        <f t="shared" ca="1" si="1"/>
-        <v>28082</v>
-      </c>
-      <c r="J9">
-        <f t="shared" ca="1" si="1"/>
-        <v>21024</v>
-      </c>
       <c r="K9">
         <f t="shared" ca="1" si="1"/>
-        <v>81397</v>
+        <v>18125</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="1"/>
-        <v>45686</v>
+        <v>55203</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="1"/>
-        <v>83698</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>61262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>22072</v>
+        <v>69238</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>49875</v>
+        <v>43120</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>74902</v>
+        <v>24167</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>20988</v>
+        <v>8386</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>12338</v>
+        <v>68954</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>86591</v>
+        <v>8413</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>86809</v>
+        <v>1325</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="1"/>
-        <v>89416</v>
+        <v>21354</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="1"/>
-        <v>25045</v>
+        <v>82036</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="1"/>
-        <v>61456</v>
+        <v>96827</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="1"/>
-        <v>55214</v>
+        <v>91825</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="1"/>
-        <v>75466</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6492</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>9932</v>
+        <v>81583</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>35197</v>
+        <v>85073</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>34445</v>
+        <v>7024</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>43135</v>
+        <v>66731</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="1"/>
-        <v>26875</v>
+        <v>29193</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>5673</v>
+        <v>56559</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>11644</v>
+        <v>58586</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="1"/>
-        <v>67327</v>
+        <v>16906</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="1"/>
-        <v>54615</v>
+        <v>88206</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="1"/>
-        <v>91831</v>
+        <v>61547</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="1"/>
-        <v>22646</v>
+        <v>84678</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="1"/>
-        <v>62675</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>59815</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>80509</v>
+        <v>64728</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>19059</v>
+        <v>35289</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>7104</v>
+        <v>90649</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>32221</v>
+        <v>66050</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
-        <v>63045</v>
+        <v>70365</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>97923</v>
+        <v>4047</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>76818</v>
+        <v>71352</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="1"/>
-        <v>53372</v>
+        <v>19470</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="1"/>
-        <v>8477</v>
+        <v>88640</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="1"/>
-        <v>87166</v>
+        <v>69843</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="1"/>
-        <v>5154</v>
+        <v>9962</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="1"/>
-        <v>38196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>67908</v>
+        <v>60995</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>7306</v>
+        <v>10061</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>70090</v>
+        <v>81390</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>28847</v>
+        <v>90307</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
-        <v>15183</v>
+        <v>4287</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>47013</v>
+        <v>86922</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>84268</v>
+        <v>92981</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="1"/>
-        <v>52202</v>
+        <v>87837</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="1"/>
-        <v>9441</v>
+        <v>69695</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="1"/>
-        <v>89011</v>
+        <v>3189</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="1"/>
-        <v>96049</v>
+        <v>21598</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="1"/>
-        <v>41767</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>69512</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>41954</v>
+        <v>81522</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>97968</v>
+        <v>71176</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>11044</v>
+        <v>79363</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>80116</v>
+        <v>81188</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
-        <v>52326</v>
+        <v>11968</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>63587</v>
+        <v>27437</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>95247</v>
+        <v>49982</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="1"/>
-        <v>19449</v>
+        <v>76483</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="1"/>
-        <v>24078</v>
+        <v>11202</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="1"/>
-        <v>56519</v>
+        <v>82124</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="1"/>
-        <v>6235</v>
+        <v>9463</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="1"/>
-        <v>25921</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>83123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>88053</v>
+        <v>33344</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>60402</v>
+        <v>4764</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>85886</v>
+        <v>29363</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>73247</v>
+        <v>39021</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="1"/>
-        <v>17230</v>
+        <v>87826</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="1"/>
-        <v>47151</v>
+        <v>83194</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>74289</v>
+        <v>92525</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="1"/>
-        <v>43270</v>
+        <v>53333</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="1"/>
-        <v>86106</v>
+        <v>12815</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="1"/>
-        <v>21469</v>
+        <v>1118</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="1"/>
-        <v>55325</v>
+        <v>97702</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="1"/>
-        <v>7042</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>26130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>54173</v>
+        <v>21344</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>26979</v>
+        <v>18594</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>52904</v>
+        <v>69986</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>49344</v>
+        <v>50431</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="1"/>
-        <v>84217</v>
+        <v>75093</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>69400</v>
+        <v>99988</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>31924</v>
+        <v>89778</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="1"/>
-        <v>90473</v>
+        <v>70450</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="1"/>
-        <v>65630</v>
+        <v>49135</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="1"/>
-        <v>3983</v>
+        <v>18979</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="1"/>
-        <v>45844</v>
+        <v>95912</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="1"/>
-        <v>24305</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>24915</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>87325</v>
+        <v>52010</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>94475</v>
+        <v>62801</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>86582</v>
+        <v>89</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>19921</v>
+        <v>35943</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>34379</v>
+        <v>62205</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>22994</v>
+        <v>78001</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>25412</v>
+        <v>76666</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>33134</v>
+        <v>26221</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>58754</v>
+        <v>3042</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
-        <v>10061</v>
+        <v>40839</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="1"/>
-        <v>61970</v>
+        <v>99446</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="1"/>
-        <v>88989</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>88017</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>27232</v>
+        <v>37352</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>69188</v>
+        <v>71870</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>51688</v>
+        <v>36264</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>3828</v>
+        <v>85873</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>78583</v>
+        <v>96508</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>72566</v>
+        <v>96250</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>22160</v>
+        <v>15907</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>60494</v>
+        <v>1961</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>56503</v>
+        <v>65587</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="1"/>
-        <v>68432</v>
+        <v>21496</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="1"/>
-        <v>59206</v>
+        <v>86798</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="1"/>
-        <v>16358</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>28530</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>78965</v>
+        <v>7022</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>60609</v>
+        <v>93454</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>62168</v>
+        <v>56031</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>67879</v>
+        <v>45299</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>28495</v>
+        <v>38875</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>69240</v>
+        <v>66371</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>30025</v>
+        <v>38355</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>4444</v>
+        <v>21872</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>70409</v>
+        <v>12001</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="1"/>
-        <v>24871</v>
+        <v>79913</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="1"/>
-        <v>53649</v>
+        <v>44389</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="1"/>
-        <v>85925</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>40835</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>32477</v>
+        <v>38115</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>30047</v>
+        <v>35416</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>72575</v>
+        <v>16180</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>38347</v>
+        <v>19807</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>90330</v>
+        <v>38897</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>83245</v>
+        <v>67157</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>89867</v>
+        <v>60229</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>69338</v>
+        <v>31171</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>46044</v>
+        <v>21470</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="1"/>
-        <v>74532</v>
+        <v>28068</v>
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="1"/>
-        <v>5554</v>
+        <v>33422</v>
       </c>
       <c r="M20">
         <f t="shared" ca="1" si="1"/>
-        <v>18657</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>23704</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>24949</v>
+        <v>14712</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>56991</v>
+        <v>53674</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>70325</v>
+        <v>5749</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>65562</v>
+        <v>48507</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>80275</v>
+        <v>66692</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>2406</v>
+        <v>76277</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>96629</v>
+        <v>3585</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>84444</v>
+        <v>36886</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>60106</v>
+        <v>50367</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="1"/>
-        <v>98021</v>
+        <v>38432</v>
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="1"/>
-        <v>75328</v>
+        <v>93746</v>
       </c>
       <c r="M21">
         <f t="shared" ca="1" si="1"/>
-        <v>76970</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>89754</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>80350</v>
+        <v>32401</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>2505</v>
+        <v>70523</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>16177</v>
+        <v>66338</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>74403</v>
+        <v>76045</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>21719</v>
+        <v>24899</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>54989</v>
+        <v>95357</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>89209</v>
+        <v>19503</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>4218</v>
+        <v>96253</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>65523</v>
+        <v>61628</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="1"/>
-        <v>68918</v>
+        <v>23531</v>
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="1"/>
-        <v>79983</v>
+        <v>32098</v>
       </c>
       <c r="M22">
         <f t="shared" ca="1" si="1"/>
-        <v>4906</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>60087</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>19920</v>
+        <v>56456</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>50425</v>
+        <v>43281</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>80323</v>
+        <v>11202</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>25287</v>
+        <v>94665</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>38315</v>
+        <v>20687</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>58003</v>
+        <v>516</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>28098</v>
+        <v>13313</v>
       </c>
       <c r="I23">
         <f t="shared" ref="C23:M31" ca="1" si="2">RANDBETWEEN(0,100000)</f>
-        <v>64666</v>
+        <v>39314</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="2"/>
-        <v>96027</v>
+        <v>77070</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="2"/>
-        <v>47385</v>
+        <v>61650</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="2"/>
-        <v>76759</v>
+        <v>44405</v>
       </c>
       <c r="M23">
         <f t="shared" ca="1" si="2"/>
-        <v>21053</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>13061</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>59623</v>
+        <v>34161</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="2"/>
-        <v>36072</v>
+        <v>64384</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="2"/>
-        <v>28360</v>
+        <v>7917</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="2"/>
-        <v>87535</v>
+        <v>90761</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="2"/>
-        <v>93288</v>
+        <v>29934</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="2"/>
-        <v>12441</v>
+        <v>5090</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
-        <v>85474</v>
+        <v>10992</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
-        <v>56503</v>
+        <v>8647</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="2"/>
-        <v>20283</v>
+        <v>66790</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="2"/>
-        <v>58048</v>
+        <v>59476</v>
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="2"/>
-        <v>66793</v>
+        <v>49471</v>
       </c>
       <c r="M24">
         <f t="shared" ca="1" si="2"/>
-        <v>39355</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>96420</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>80109</v>
+        <v>70620</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="2"/>
-        <v>97521</v>
+        <v>48329</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="2"/>
-        <v>89712</v>
+        <v>91745</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="2"/>
-        <v>42848</v>
+        <v>24732</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="2"/>
-        <v>12384</v>
+        <v>35284</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="2"/>
-        <v>48547</v>
+        <v>18257</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
-        <v>80056</v>
+        <v>29239</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
-        <v>58482</v>
+        <v>4715</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="2"/>
-        <v>81853</v>
+        <v>62681</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="2"/>
-        <v>6914</v>
+        <v>94265</v>
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="2"/>
-        <v>59971</v>
+        <v>38694</v>
       </c>
       <c r="M25">
         <f t="shared" ca="1" si="2"/>
-        <v>70376</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>14660</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>11978</v>
+        <v>87238</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="2"/>
-        <v>42178</v>
+        <v>60726</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="2"/>
-        <v>51488</v>
+        <v>1953</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="2"/>
-        <v>83709</v>
+        <v>4985</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="2"/>
-        <v>1459</v>
+        <v>90867</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="2"/>
-        <v>71739</v>
+        <v>8488</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
-        <v>32516</v>
+        <v>41373</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
-        <v>72609</v>
+        <v>94383</v>
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="2"/>
-        <v>96264</v>
+        <v>16661</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="2"/>
-        <v>35045</v>
+        <v>67603</v>
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="2"/>
-        <v>47969</v>
+        <v>41104</v>
       </c>
       <c r="M26">
         <f t="shared" ca="1" si="2"/>
-        <v>66469</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>47889</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>58272</v>
+        <v>13140</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="2"/>
-        <v>28086</v>
+        <v>18258</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="2"/>
-        <v>87986</v>
+        <v>65194</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="2"/>
-        <v>13174</v>
+        <v>15507</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="2"/>
-        <v>22315</v>
+        <v>89545</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="2"/>
-        <v>14217</v>
+        <v>55344</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>71362</v>
+        <v>76853</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
-        <v>93951</v>
+        <v>23854</v>
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="2"/>
-        <v>57805</v>
+        <v>59077</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="2"/>
-        <v>50599</v>
+        <v>18986</v>
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="2"/>
-        <v>6332</v>
+        <v>69950</v>
       </c>
       <c r="M27">
         <f t="shared" ca="1" si="2"/>
-        <v>94162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>15031</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>67979</v>
+        <v>95058</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="2"/>
-        <v>98838</v>
+        <v>78535</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="2"/>
-        <v>49019</v>
+        <v>69871</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="2"/>
-        <v>51366</v>
+        <v>19553</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="2"/>
-        <v>34806</v>
+        <v>56923</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="2"/>
-        <v>88793</v>
+        <v>46746</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>60090</v>
+        <v>77382</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
-        <v>55546</v>
+        <v>27846</v>
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="2"/>
-        <v>4145</v>
+        <v>8538</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="2"/>
-        <v>8097</v>
+        <v>59866</v>
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="2"/>
-        <v>48434</v>
+        <v>44407</v>
       </c>
       <c r="M28">
         <f t="shared" ca="1" si="2"/>
-        <v>7541</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>46899</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>94567</v>
+        <v>4439</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="2"/>
-        <v>73176</v>
+        <v>80217</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="2"/>
-        <v>22118</v>
+        <v>38423</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="2"/>
-        <v>83704</v>
+        <v>4970</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="2"/>
-        <v>23360</v>
+        <v>93743</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="2"/>
-        <v>17762</v>
+        <v>43688</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
-        <v>80710</v>
+        <v>58471</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="2"/>
-        <v>16391</v>
+        <v>87123</v>
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="2"/>
-        <v>42297</v>
+        <v>16702</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="2"/>
-        <v>84449</v>
+        <v>72578</v>
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="2"/>
-        <v>45999</v>
+        <v>78829</v>
       </c>
       <c r="M29">
         <f t="shared" ca="1" si="2"/>
-        <v>45248</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>40</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>13433</v>
+        <v>24432</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="2"/>
-        <v>44292</v>
+        <v>37612</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="2"/>
-        <v>30402</v>
+        <v>4185</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="2"/>
-        <v>4235</v>
+        <v>57430</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="2"/>
-        <v>48680</v>
+        <v>73387</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="2"/>
-        <v>6564</v>
+        <v>42503</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
-        <v>72215</v>
+        <v>58687</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="2"/>
-        <v>82051</v>
+        <v>35430</v>
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="2"/>
-        <v>74493</v>
+        <v>76167</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="2"/>
-        <v>57324</v>
+        <v>29866</v>
       </c>
       <c r="L30">
         <f t="shared" ca="1" si="2"/>
-        <v>94949</v>
+        <v>56614</v>
       </c>
       <c r="M30">
         <f t="shared" ca="1" si="2"/>
-        <v>75557</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>90073</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>41</v>
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="1"/>
-        <v>34032</v>
+        <v>14455</v>
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="2"/>
-        <v>44873</v>
+        <v>59429</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="2"/>
-        <v>83018</v>
+        <v>95858</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="2"/>
-        <v>735</v>
+        <v>89456</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="2"/>
-        <v>95854</v>
+        <v>28538</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="2"/>
-        <v>64290</v>
+        <v>69021</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
-        <v>29409</v>
+        <v>83731</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="2"/>
-        <v>86597</v>
+        <v>61111</v>
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="2"/>
-        <v>51464</v>
+        <v>50410</v>
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="2"/>
-        <v>12828</v>
+        <v>37436</v>
       </c>
       <c r="L31">
         <f t="shared" ca="1" si="2"/>
-        <v>93069</v>
+        <v>68725</v>
       </c>
       <c r="M31">
         <f t="shared" ca="1" si="2"/>
-        <v>88541</v>
+        <v>88867</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tables now loads from server & added some optimization
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC0BADF-508F-4049-AB8F-5025E72C4FF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39E7FEA-B782-4F8E-88F6-A41CEC781E86}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Тестовый отдел" sheetId="1" r:id="rId1"/>
+    <sheet name="Отдел для тестов" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист, лист, лист" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
   <si>
     <t>январь</t>
   </si>
@@ -146,6 +148,69 @@
   </si>
   <si>
     <t>к30</t>
+  </si>
+  <si>
+    <t>один</t>
+  </si>
+  <si>
+    <t>два</t>
+  </si>
+  <si>
+    <t>три</t>
+  </si>
+  <si>
+    <t>четыре</t>
+  </si>
+  <si>
+    <t>пять</t>
+  </si>
+  <si>
+    <t>шесть</t>
+  </si>
+  <si>
+    <t>семь</t>
+  </si>
+  <si>
+    <t>восемь</t>
+  </si>
+  <si>
+    <t>девять</t>
+  </si>
+  <si>
+    <t>десять</t>
+  </si>
+  <si>
+    <t>одиннацадь</t>
+  </si>
+  <si>
+    <t>двеннадцать</t>
+  </si>
+  <si>
+    <t>тринадцать</t>
+  </si>
+  <si>
+    <t>четырнацать</t>
+  </si>
+  <si>
+    <t>слово</t>
+  </si>
+  <si>
+    <t>ещё одно</t>
+  </si>
+  <si>
+    <t>и ещё</t>
+  </si>
+  <si>
+    <t>и снова</t>
+  </si>
+  <si>
+    <t>больше слов</t>
+  </si>
+  <si>
+    <t>словаааа</t>
+  </si>
+  <si>
+    <t>хех</t>
   </si>
 </sst>
 </file>
@@ -465,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,51 +580,51 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(0,100000)</f>
-        <v>6571</v>
+        <v>94992</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:M2" ca="1" si="0">RANDBETWEEN(0,100000)</f>
-        <v>37829</v>
+        <v>62741</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>81348</v>
+        <v>56361</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>71395</v>
+        <v>12267</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>90533</v>
+        <v>19892</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>7402</v>
+        <v>17351</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>66895</v>
+        <v>42192</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>42083</v>
+        <v>21515</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>84861</v>
+        <v>79426</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>25087</v>
+        <v>2803</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>73797</v>
+        <v>55356</v>
       </c>
       <c r="M2">
         <f t="shared" ca="1" si="0"/>
-        <v>52934</v>
+        <v>48041</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -568,51 +633,51 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:M31" ca="1" si="1">RANDBETWEEN(0,100000)</f>
-        <v>95867</v>
+        <v>89352</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>6611</v>
+        <v>41316</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>45109</v>
+        <v>64624</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>80210</v>
+        <v>21464</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>40128</v>
+        <v>63407</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>96737</v>
+        <v>90477</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>40426</v>
+        <v>3006</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="1"/>
-        <v>82588</v>
+        <v>2664</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="1"/>
-        <v>55402</v>
+        <v>21664</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="1"/>
-        <v>51551</v>
+        <v>73002</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="1"/>
-        <v>28583</v>
+        <v>54483</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="1"/>
-        <v>88121</v>
+        <v>81507</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -621,51 +686,51 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>30919</v>
+        <v>80342</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>78329</v>
+        <v>41387</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>140</v>
+        <v>8537</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>19828</v>
+        <v>35909</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>42686</v>
+        <v>74765</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>98021</v>
+        <v>34536</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>92582</v>
+        <v>30099</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="1"/>
-        <v>16444</v>
+        <v>79286</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="1"/>
-        <v>80979</v>
+        <v>3491</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="1"/>
-        <v>11268</v>
+        <v>94516</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="1"/>
-        <v>7582</v>
+        <v>45701</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="1"/>
-        <v>74035</v>
+        <v>74950</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -674,51 +739,51 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>36380</v>
+        <v>57904</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>55895</v>
+        <v>29383</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>34421</v>
+        <v>25047</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>58419</v>
+        <v>4469</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>1518</v>
+        <v>9519</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>31334</v>
+        <v>74737</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>70036</v>
+        <v>20737</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="1"/>
-        <v>66929</v>
+        <v>75832</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="1"/>
-        <v>6455</v>
+        <v>89439</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="1"/>
-        <v>55187</v>
+        <v>21949</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="1"/>
-        <v>565</v>
+        <v>69068</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="1"/>
-        <v>9832</v>
+        <v>85946</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -727,51 +792,51 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>66703</v>
+        <v>28555</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>49131</v>
+        <v>27810</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>35620</v>
+        <v>11657</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>78681</v>
+        <v>32056</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>42473</v>
+        <v>63263</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>95219</v>
+        <v>35608</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>80083</v>
+        <v>35045</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="1"/>
-        <v>10481</v>
+        <v>86630</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="1"/>
-        <v>50044</v>
+        <v>60212</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="1"/>
-        <v>32647</v>
+        <v>27605</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="1"/>
-        <v>43196</v>
+        <v>15515</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="1"/>
-        <v>3383</v>
+        <v>24255</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -780,51 +845,51 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>69908</v>
+        <v>67781</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>52906</v>
+        <v>79494</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>43976</v>
+        <v>40981</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>58760</v>
+        <v>31944</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>96108</v>
+        <v>60893</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>43225</v>
+        <v>51427</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>10395</v>
+        <v>11364</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="1"/>
-        <v>22582</v>
+        <v>64734</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>77978</v>
+        <v>47605</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="1"/>
-        <v>66699</v>
+        <v>65315</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="1"/>
-        <v>89085</v>
+        <v>92466</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="1"/>
-        <v>59836</v>
+        <v>2441</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -833,51 +898,51 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>81465</v>
+        <v>45172</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>5495</v>
+        <v>85270</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>81244</v>
+        <v>88968</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>64285</v>
+        <v>78015</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>20734</v>
+        <v>90083</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>53085</v>
+        <v>48522</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>64279</v>
+        <v>84353</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="1"/>
-        <v>86060</v>
+        <v>63035</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="1"/>
-        <v>54952</v>
+        <v>58967</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="1"/>
-        <v>64302</v>
+        <v>90057</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="1"/>
-        <v>80672</v>
+        <v>54875</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="1"/>
-        <v>41337</v>
+        <v>56591</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -886,51 +951,51 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>55017</v>
+        <v>65882</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>14321</v>
+        <v>77846</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>86684</v>
+        <v>96163</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>69946</v>
+        <v>83333</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>50853</v>
+        <v>47283</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
-        <v>81153</v>
+        <v>36116</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>6693</v>
+        <v>56718</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="1"/>
-        <v>13046</v>
+        <v>20435</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="1"/>
-        <v>12013</v>
+        <v>43519</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="1"/>
-        <v>18125</v>
+        <v>5227</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="1"/>
-        <v>55203</v>
+        <v>44700</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="1"/>
-        <v>61262</v>
+        <v>27655</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -939,51 +1004,51 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>69238</v>
+        <v>46816</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>43120</v>
+        <v>38308</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>24167</v>
+        <v>9692</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>8386</v>
+        <v>26477</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>68954</v>
+        <v>42025</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>8413</v>
+        <v>46074</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>1325</v>
+        <v>54071</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="1"/>
-        <v>21354</v>
+        <v>83695</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="1"/>
-        <v>82036</v>
+        <v>95817</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="1"/>
-        <v>96827</v>
+        <v>51477</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="1"/>
-        <v>91825</v>
+        <v>43097</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="1"/>
-        <v>6492</v>
+        <v>56494</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -992,51 +1057,51 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>81583</v>
+        <v>46264</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>85073</v>
+        <v>59622</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>7024</v>
+        <v>14013</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>66731</v>
+        <v>9916</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="1"/>
-        <v>29193</v>
+        <v>35655</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>56559</v>
+        <v>80149</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>58586</v>
+        <v>26312</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="1"/>
-        <v>16906</v>
+        <v>89822</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="1"/>
-        <v>88206</v>
+        <v>94696</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="1"/>
-        <v>61547</v>
+        <v>10126</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="1"/>
-        <v>84678</v>
+        <v>43446</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="1"/>
-        <v>59815</v>
+        <v>96739</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1045,51 +1110,51 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>64728</v>
+        <v>32875</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>35289</v>
+        <v>64998</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>90649</v>
+        <v>62099</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>66050</v>
+        <v>16080</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
-        <v>70365</v>
+        <v>13076</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>4047</v>
+        <v>85425</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>71352</v>
+        <v>82805</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="1"/>
-        <v>19470</v>
+        <v>61056</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="1"/>
-        <v>88640</v>
+        <v>39872</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="1"/>
-        <v>69843</v>
+        <v>83603</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="1"/>
-        <v>9962</v>
+        <v>13089</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="1"/>
-        <v>11377</v>
+        <v>83432</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1098,51 +1163,51 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>60995</v>
+        <v>81972</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>10061</v>
+        <v>95457</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>81390</v>
+        <v>47887</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>90307</v>
+        <v>38532</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
-        <v>4287</v>
+        <v>35144</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>86922</v>
+        <v>10722</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>92981</v>
+        <v>983</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="1"/>
-        <v>87837</v>
+        <v>62128</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="1"/>
-        <v>69695</v>
+        <v>79816</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="1"/>
-        <v>3189</v>
+        <v>75426</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="1"/>
-        <v>21598</v>
+        <v>63040</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="1"/>
-        <v>69512</v>
+        <v>26831</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1151,51 +1216,51 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>81522</v>
+        <v>73292</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>71176</v>
+        <v>37179</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>79363</v>
+        <v>67469</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>81188</v>
+        <v>28987</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
-        <v>11968</v>
+        <v>61580</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>27437</v>
+        <v>70521</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>49982</v>
+        <v>16011</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="1"/>
-        <v>76483</v>
+        <v>66676</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="1"/>
-        <v>11202</v>
+        <v>19245</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="1"/>
-        <v>82124</v>
+        <v>73168</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="1"/>
-        <v>9463</v>
+        <v>66274</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="1"/>
-        <v>83123</v>
+        <v>85119</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1204,51 +1269,51 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>33344</v>
+        <v>43736</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>4764</v>
+        <v>86494</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>29363</v>
+        <v>84271</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>39021</v>
+        <v>91142</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="1"/>
-        <v>87826</v>
+        <v>62044</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="1"/>
-        <v>83194</v>
+        <v>22972</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>92525</v>
+        <v>52084</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="1"/>
-        <v>53333</v>
+        <v>91838</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="1"/>
-        <v>12815</v>
+        <v>92640</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="1"/>
-        <v>1118</v>
+        <v>1332</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="1"/>
-        <v>97702</v>
+        <v>56350</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="1"/>
-        <v>26130</v>
+        <v>70732</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1257,51 +1322,51 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>21344</v>
+        <v>25876</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>18594</v>
+        <v>6511</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>69986</v>
+        <v>49634</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>50431</v>
+        <v>89149</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="1"/>
-        <v>75093</v>
+        <v>32968</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>99988</v>
+        <v>89413</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>89778</v>
+        <v>11537</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="1"/>
-        <v>70450</v>
+        <v>30027</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="1"/>
-        <v>49135</v>
+        <v>11652</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="1"/>
-        <v>18979</v>
+        <v>77141</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="1"/>
-        <v>95912</v>
+        <v>43805</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="1"/>
-        <v>24915</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1310,51 +1375,51 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>52010</v>
+        <v>23990</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>62801</v>
+        <v>98952</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>89</v>
+        <v>84620</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>35943</v>
+        <v>96175</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>62205</v>
+        <v>5670</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>78001</v>
+        <v>62138</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>76666</v>
+        <v>51733</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>26221</v>
+        <v>66421</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>3042</v>
+        <v>87069</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
-        <v>40839</v>
+        <v>48241</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="1"/>
-        <v>99446</v>
+        <v>95260</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="1"/>
-        <v>88017</v>
+        <v>68423</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1363,51 +1428,51 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>37352</v>
+        <v>38242</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>71870</v>
+        <v>8348</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>36264</v>
+        <v>22136</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>85873</v>
+        <v>43545</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>96508</v>
+        <v>12235</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>96250</v>
+        <v>53933</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>15907</v>
+        <v>97054</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>1961</v>
+        <v>3416</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>65587</v>
+        <v>75401</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="1"/>
-        <v>21496</v>
+        <v>51214</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="1"/>
-        <v>86798</v>
+        <v>78046</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="1"/>
-        <v>28530</v>
+        <v>92450</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1416,51 +1481,51 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>7022</v>
+        <v>79629</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>93454</v>
+        <v>52946</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>56031</v>
+        <v>37081</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>45299</v>
+        <v>49680</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>38875</v>
+        <v>8697</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>66371</v>
+        <v>77102</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>38355</v>
+        <v>80264</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>21872</v>
+        <v>9070</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>12001</v>
+        <v>79078</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="1"/>
-        <v>79913</v>
+        <v>83738</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="1"/>
-        <v>44389</v>
+        <v>98057</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="1"/>
-        <v>40835</v>
+        <v>18587</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1469,51 +1534,51 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>38115</v>
+        <v>6227</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>35416</v>
+        <v>83513</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>16180</v>
+        <v>1682</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>19807</v>
+        <v>44437</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>38897</v>
+        <v>93490</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>67157</v>
+        <v>42810</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>60229</v>
+        <v>17924</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>31171</v>
+        <v>93351</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>21470</v>
+        <v>92378</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="1"/>
-        <v>28068</v>
+        <v>93778</v>
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="1"/>
-        <v>33422</v>
+        <v>26979</v>
       </c>
       <c r="M20">
         <f t="shared" ca="1" si="1"/>
-        <v>23704</v>
+        <v>11132</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1522,51 +1587,51 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>14712</v>
+        <v>96467</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>53674</v>
+        <v>99855</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>5749</v>
+        <v>37808</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>48507</v>
+        <v>63594</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>66692</v>
+        <v>86231</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>76277</v>
+        <v>34255</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>3585</v>
+        <v>85060</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>36886</v>
+        <v>61212</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>50367</v>
+        <v>60678</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="1"/>
-        <v>38432</v>
+        <v>28581</v>
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="1"/>
-        <v>93746</v>
+        <v>84174</v>
       </c>
       <c r="M21">
         <f t="shared" ca="1" si="1"/>
-        <v>89754</v>
+        <v>22509</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -1575,51 +1640,51 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>32401</v>
+        <v>96587</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>70523</v>
+        <v>66685</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>66338</v>
+        <v>76072</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>76045</v>
+        <v>13294</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>24899</v>
+        <v>75344</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>95357</v>
+        <v>23734</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>19503</v>
+        <v>46602</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>96253</v>
+        <v>9978</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>61628</v>
+        <v>30768</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="1"/>
-        <v>23531</v>
+        <v>9339</v>
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="1"/>
-        <v>32098</v>
+        <v>56170</v>
       </c>
       <c r="M22">
         <f t="shared" ca="1" si="1"/>
-        <v>60087</v>
+        <v>7086</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -1628,51 +1693,51 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>56456</v>
+        <v>16220</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>43281</v>
+        <v>71342</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>11202</v>
+        <v>83441</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>94665</v>
+        <v>57778</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>20687</v>
+        <v>97941</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>516</v>
+        <v>61308</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>13313</v>
+        <v>45606</v>
       </c>
       <c r="I23">
         <f t="shared" ref="C23:M31" ca="1" si="2">RANDBETWEEN(0,100000)</f>
-        <v>39314</v>
+        <v>93648</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="2"/>
-        <v>77070</v>
+        <v>31313</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="2"/>
-        <v>61650</v>
+        <v>56555</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="2"/>
-        <v>44405</v>
+        <v>29065</v>
       </c>
       <c r="M23">
         <f t="shared" ca="1" si="2"/>
-        <v>13061</v>
+        <v>78815</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -1681,51 +1746,51 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>34161</v>
+        <v>78147</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="2"/>
-        <v>64384</v>
+        <v>13970</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="2"/>
-        <v>7917</v>
+        <v>15687</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="2"/>
-        <v>90761</v>
+        <v>15919</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="2"/>
-        <v>29934</v>
+        <v>47632</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="2"/>
-        <v>5090</v>
+        <v>44443</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
-        <v>10992</v>
+        <v>92422</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
-        <v>8647</v>
+        <v>98169</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="2"/>
-        <v>66790</v>
+        <v>40549</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="2"/>
-        <v>59476</v>
+        <v>88708</v>
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="2"/>
-        <v>49471</v>
+        <v>96783</v>
       </c>
       <c r="M24">
         <f t="shared" ca="1" si="2"/>
-        <v>96420</v>
+        <v>37553</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -1734,51 +1799,51 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>70620</v>
+        <v>60630</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="2"/>
-        <v>48329</v>
+        <v>90637</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="2"/>
-        <v>91745</v>
+        <v>5027</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="2"/>
-        <v>24732</v>
+        <v>62371</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="2"/>
-        <v>35284</v>
+        <v>60882</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="2"/>
-        <v>18257</v>
+        <v>9189</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
-        <v>29239</v>
+        <v>6758</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
-        <v>4715</v>
+        <v>73585</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="2"/>
-        <v>62681</v>
+        <v>97627</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="2"/>
-        <v>94265</v>
+        <v>78137</v>
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="2"/>
-        <v>38694</v>
+        <v>53174</v>
       </c>
       <c r="M25">
         <f t="shared" ca="1" si="2"/>
-        <v>14660</v>
+        <v>95420</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -1787,51 +1852,51 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>87238</v>
+        <v>81272</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="2"/>
-        <v>60726</v>
+        <v>49720</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="2"/>
-        <v>1953</v>
+        <v>30076</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="2"/>
-        <v>4985</v>
+        <v>81752</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="2"/>
-        <v>90867</v>
+        <v>6536</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="2"/>
-        <v>8488</v>
+        <v>85494</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
-        <v>41373</v>
+        <v>32506</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
-        <v>94383</v>
+        <v>6815</v>
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="2"/>
-        <v>16661</v>
+        <v>69471</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="2"/>
-        <v>67603</v>
+        <v>37742</v>
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="2"/>
-        <v>41104</v>
+        <v>97745</v>
       </c>
       <c r="M26">
         <f t="shared" ca="1" si="2"/>
-        <v>47889</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -1840,51 +1905,51 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>13140</v>
+        <v>32346</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="2"/>
-        <v>18258</v>
+        <v>16277</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="2"/>
-        <v>65194</v>
+        <v>12105</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="2"/>
-        <v>15507</v>
+        <v>16310</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="2"/>
-        <v>89545</v>
+        <v>84344</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="2"/>
-        <v>55344</v>
+        <v>55763</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>76853</v>
+        <v>59928</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
-        <v>23854</v>
+        <v>77782</v>
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="2"/>
-        <v>59077</v>
+        <v>15882</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="2"/>
-        <v>18986</v>
+        <v>71799</v>
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="2"/>
-        <v>69950</v>
+        <v>35711</v>
       </c>
       <c r="M27">
         <f t="shared" ca="1" si="2"/>
-        <v>15031</v>
+        <v>69979</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -1893,51 +1958,51 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>95058</v>
+        <v>29952</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="2"/>
-        <v>78535</v>
+        <v>99801</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="2"/>
-        <v>69871</v>
+        <v>49197</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="2"/>
-        <v>19553</v>
+        <v>30058</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="2"/>
-        <v>56923</v>
+        <v>63964</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="2"/>
-        <v>46746</v>
+        <v>6496</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>77382</v>
+        <v>31020</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
-        <v>27846</v>
+        <v>96139</v>
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="2"/>
-        <v>8538</v>
+        <v>52289</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="2"/>
-        <v>59866</v>
+        <v>66872</v>
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="2"/>
-        <v>44407</v>
+        <v>56387</v>
       </c>
       <c r="M28">
         <f t="shared" ca="1" si="2"/>
-        <v>46899</v>
+        <v>18587</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -1946,51 +2011,51 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>4439</v>
+        <v>74751</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="2"/>
-        <v>80217</v>
+        <v>25290</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="2"/>
-        <v>38423</v>
+        <v>47456</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="2"/>
-        <v>4970</v>
+        <v>371</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="2"/>
-        <v>93743</v>
+        <v>52885</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="2"/>
-        <v>43688</v>
+        <v>42428</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
-        <v>58471</v>
+        <v>99290</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="2"/>
-        <v>87123</v>
+        <v>53596</v>
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="2"/>
-        <v>16702</v>
+        <v>93539</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="2"/>
-        <v>72578</v>
+        <v>48276</v>
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="2"/>
-        <v>78829</v>
+        <v>77950</v>
       </c>
       <c r="M29">
         <f t="shared" ca="1" si="2"/>
-        <v>1591</v>
+        <v>6257</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -1999,51 +2064,51 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>24432</v>
+        <v>11778</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="2"/>
-        <v>37612</v>
+        <v>21702</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="2"/>
-        <v>4185</v>
+        <v>47165</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="2"/>
-        <v>57430</v>
+        <v>52152</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="2"/>
-        <v>73387</v>
+        <v>96957</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="2"/>
-        <v>42503</v>
+        <v>26157</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
-        <v>58687</v>
+        <v>23282</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="2"/>
-        <v>35430</v>
+        <v>80262</v>
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="2"/>
-        <v>76167</v>
+        <v>61124</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="2"/>
-        <v>29866</v>
+        <v>26600</v>
       </c>
       <c r="L30">
         <f t="shared" ca="1" si="2"/>
-        <v>56614</v>
+        <v>71128</v>
       </c>
       <c r="M30">
         <f t="shared" ca="1" si="2"/>
-        <v>90073</v>
+        <v>84603</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -2052,55 +2117,1327 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="1"/>
-        <v>14455</v>
+        <v>53169</v>
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="2"/>
-        <v>59429</v>
+        <v>85141</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="2"/>
-        <v>95858</v>
+        <v>65589</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="2"/>
-        <v>89456</v>
+        <v>36313</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="2"/>
-        <v>28538</v>
+        <v>18075</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="2"/>
-        <v>69021</v>
+        <v>98209</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
-        <v>83731</v>
+        <v>26901</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="2"/>
-        <v>61111</v>
+        <v>57920</v>
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="2"/>
-        <v>50410</v>
+        <v>9958</v>
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="2"/>
-        <v>37436</v>
+        <v>29521</v>
       </c>
       <c r="L31">
         <f t="shared" ca="1" si="2"/>
-        <v>68725</v>
+        <v>86693</v>
       </c>
       <c r="M31">
         <f t="shared" ca="1" si="2"/>
-        <v>88867</v>
+        <v>746</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2443DA-52F3-41DE-A514-0CCB55DF48B8}">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <f ca="1">RANDBETWEEN(1000, 2000)</f>
+        <v>1625</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:M15" ca="1" si="0">RANDBETWEEN(1000, 2000)</f>
+        <v>1028</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1530</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1133</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1926</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1289</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1688</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1334</v>
+      </c>
+      <c r="J2">
+        <f ca="1">RANDBETWEEN(1000, 2000)</f>
+        <v>1527</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1238</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1753</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B15" ca="1" si="1">RANDBETWEEN(1000, 2000)</f>
+        <v>1204</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1710</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1709</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1316</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1321</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1195</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1484</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1610</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1651</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1359</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1048</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1341</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1872</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1421</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1032</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1860</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1393</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1236</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1209</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1412</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1551</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1546</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1938</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1083</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1143</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1212</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1951</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1826</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1296</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1544</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1728</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1299</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1397</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1155</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1499</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1530</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1187</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1040</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1076</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1407</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1617</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1794</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1910</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1329</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1301</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1992</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1525</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1963</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1106</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1105</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1931</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1020</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1760</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1891</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1365</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1951</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1513</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1223</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1514</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1338</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1795</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1931</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1516</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1377</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1536</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="1"/>
+        <v>1421</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1913</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1445</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1567</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1373</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1222</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1276</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1754</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1433</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1549</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1991</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="1"/>
+        <v>1603</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1658</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1647</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1823</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1416</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1706</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1691</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1420</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1987</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1624</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1774</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="1"/>
+        <v>1614</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1505</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1702</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1091</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1593</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1351</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1114</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1747</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1479</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1974</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1566</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="1"/>
+        <v>1307</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1947</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1603</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1841</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1730</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1434</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1424</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1669</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1775</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1199</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1289</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="1"/>
+        <v>1298</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1845</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1011</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1960</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1994</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1072</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1613</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1488</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1353</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1188</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1296</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="1"/>
+        <v>1969</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1837</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1632</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1360</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1331</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1571</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1029</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1742</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1359</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1350</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1306</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="1"/>
+        <v>1314</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1538</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1770</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1099</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1531</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1052</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1307</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1930</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1507</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1584</v>
+      </c>
+      <c r="L15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1326</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1915</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BB9E37-D208-4535-81AC-826820395CFC}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2">
+        <f ca="1">RANDBETWEEN(0,100)</f>
+        <v>75</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:M9" ca="1" si="0">RANDBETWEEN(0,100)</f>
+        <v>67</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ca="1" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B9" ca="1" si="1">RANDBETWEEN(0,100)</f>
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ca="1" si="0"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ca="1" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ca="1" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>